<commit_message>
Modifying Little Bear River data use case queries and benchmarking
</commit_message>
<xml_diff>
--- a/usecases/littlebearriver/sqlscripts/QueryBenchmarking.xlsx
+++ b/usecases/littlebearriver/sqlscripts/QueryBenchmarking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29960" yWindow="4260" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="23260" yWindow="0" windowWidth="14940" windowHeight="21680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="7">
   <si>
     <t>Query</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>ODM2 is slower</t>
-  </si>
-  <si>
-    <t>Greater than 5 minutes without series catalog…</t>
   </si>
 </sst>
 </file>
@@ -91,8 +88,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -107,17 +126,39 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J27"/>
+  <dimension ref="A2:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -900,21 +941,48 @@
       <c r="C24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" t="e">
+      <c r="D24">
+        <v>582</v>
+      </c>
+      <c r="E24">
+        <v>567</v>
+      </c>
+      <c r="F24">
+        <v>568</v>
+      </c>
+      <c r="G24">
+        <v>568</v>
+      </c>
+      <c r="H24">
+        <v>568</v>
+      </c>
+      <c r="I24">
         <f>AVERAGE(D24:H24)</f>
-        <v>#DIV/0!</v>
+        <v>570.6</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="C25" t="s">
         <v>3</v>
       </c>
-      <c r="I25" t="e">
+      <c r="D25">
+        <v>4418</v>
+      </c>
+      <c r="E25">
+        <v>4367</v>
+      </c>
+      <c r="F25">
+        <v>4383</v>
+      </c>
+      <c r="G25">
+        <v>4400</v>
+      </c>
+      <c r="H25">
+        <v>4306</v>
+      </c>
+      <c r="I25">
         <f>AVERAGE(D25:H25)</f>
-        <v>#DIV/0!</v>
+        <v>4374.8</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -965,6 +1033,1346 @@
       </c>
       <c r="I27">
         <f>AVERAGE(D27:H27)</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>928</v>
+      </c>
+      <c r="E31">
+        <v>929</v>
+      </c>
+      <c r="F31">
+        <v>928</v>
+      </c>
+      <c r="G31">
+        <v>929</v>
+      </c>
+      <c r="H31">
+        <v>930</v>
+      </c>
+      <c r="I31">
+        <f>AVERAGE(D31:H31)</f>
+        <v>928.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>7330</v>
+      </c>
+      <c r="E32">
+        <v>7334</v>
+      </c>
+      <c r="F32">
+        <v>7346</v>
+      </c>
+      <c r="G32">
+        <v>7333</v>
+      </c>
+      <c r="H32">
+        <v>7345</v>
+      </c>
+      <c r="I32">
+        <f>AVERAGE(D32:H32)</f>
+        <v>7337.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <f>AVERAGE(D33:H33)</f>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>16</v>
+      </c>
+      <c r="H34">
+        <v>15</v>
+      </c>
+      <c r="I34">
+        <f>AVERAGE(D34:H34)</f>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>931</v>
+      </c>
+      <c r="E38">
+        <v>927</v>
+      </c>
+      <c r="F38">
+        <v>928</v>
+      </c>
+      <c r="G38">
+        <v>929</v>
+      </c>
+      <c r="H38">
+        <v>929</v>
+      </c>
+      <c r="I38">
+        <f>AVERAGE(D38:H38)</f>
+        <v>928.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>7318</v>
+      </c>
+      <c r="E39">
+        <v>7345</v>
+      </c>
+      <c r="F39">
+        <v>7362</v>
+      </c>
+      <c r="G39">
+        <v>7364</v>
+      </c>
+      <c r="H39">
+        <v>7317</v>
+      </c>
+      <c r="I39">
+        <f>AVERAGE(D39:H39)</f>
+        <v>7341.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <f>AVERAGE(D40:H40)</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f>AVERAGE(D41:H41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>854</v>
+      </c>
+      <c r="E45">
+        <v>853</v>
+      </c>
+      <c r="F45">
+        <v>853</v>
+      </c>
+      <c r="G45">
+        <v>854</v>
+      </c>
+      <c r="H45">
+        <v>852</v>
+      </c>
+      <c r="I45">
+        <f>AVERAGE(D45:H45)</f>
+        <v>853.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>6773</v>
+      </c>
+      <c r="E46">
+        <v>6722</v>
+      </c>
+      <c r="F46">
+        <v>6741</v>
+      </c>
+      <c r="G46">
+        <v>6694</v>
+      </c>
+      <c r="H46">
+        <v>6723</v>
+      </c>
+      <c r="I46">
+        <f>AVERAGE(D46:H46)</f>
+        <v>6730.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>15</v>
+      </c>
+      <c r="E47">
+        <v>13</v>
+      </c>
+      <c r="F47">
+        <v>14</v>
+      </c>
+      <c r="G47">
+        <v>13</v>
+      </c>
+      <c r="H47">
+        <v>14</v>
+      </c>
+      <c r="I47">
+        <f>AVERAGE(D47:H47)</f>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>16</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+      <c r="F48">
+        <v>16</v>
+      </c>
+      <c r="G48">
+        <v>15</v>
+      </c>
+      <c r="H48">
+        <v>16</v>
+      </c>
+      <c r="I48">
+        <f>AVERAGE(D48:H48)</f>
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51" t="s">
+        <v>4</v>
+      </c>
+      <c r="J51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>89765</v>
+      </c>
+      <c r="E52">
+        <v>89800</v>
+      </c>
+      <c r="F52">
+        <v>89710</v>
+      </c>
+      <c r="G52">
+        <v>282219</v>
+      </c>
+      <c r="H52">
+        <v>278291</v>
+      </c>
+      <c r="I52">
+        <f>AVERAGE(D52:H52)</f>
+        <v>165957</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>89763</v>
+      </c>
+      <c r="E53">
+        <v>89779</v>
+      </c>
+      <c r="F53">
+        <v>89653</v>
+      </c>
+      <c r="G53">
+        <v>143302</v>
+      </c>
+      <c r="H53">
+        <v>142866</v>
+      </c>
+      <c r="I53">
+        <f>AVERAGE(D53:H53)</f>
+        <v>111072.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>234</v>
+      </c>
+      <c r="E54">
+        <v>231</v>
+      </c>
+      <c r="F54">
+        <v>227</v>
+      </c>
+      <c r="G54">
+        <v>214</v>
+      </c>
+      <c r="H54">
+        <v>214</v>
+      </c>
+      <c r="I54">
+        <f>AVERAGE(D54:H54)</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>187</v>
+      </c>
+      <c r="E55">
+        <v>124</v>
+      </c>
+      <c r="F55">
+        <v>125</v>
+      </c>
+      <c r="G55">
+        <v>156</v>
+      </c>
+      <c r="H55">
+        <v>78</v>
+      </c>
+      <c r="I55">
+        <f>AVERAGE(D55:H55)</f>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58">
+        <v>4</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58" t="s">
+        <v>4</v>
+      </c>
+      <c r="J58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59">
+        <v>9</v>
+      </c>
+      <c r="B59">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>516</v>
+      </c>
+      <c r="E59">
+        <v>517</v>
+      </c>
+      <c r="F59">
+        <v>518</v>
+      </c>
+      <c r="G59">
+        <v>518</v>
+      </c>
+      <c r="H59">
+        <v>516</v>
+      </c>
+      <c r="I59">
+        <f>AVERAGE(D59:H59)</f>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>4009</v>
+      </c>
+      <c r="E60">
+        <v>3945</v>
+      </c>
+      <c r="F60">
+        <v>3916</v>
+      </c>
+      <c r="G60">
+        <v>3997</v>
+      </c>
+      <c r="H60">
+        <v>3991</v>
+      </c>
+      <c r="I60">
+        <f>AVERAGE(D60:H60)</f>
+        <v>3971.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>3</v>
+      </c>
+      <c r="I61">
+        <f>AVERAGE(D61:H61)</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>16</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <f>AVERAGE(D62:H62)</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>524</v>
+      </c>
+      <c r="E66">
+        <v>525</v>
+      </c>
+      <c r="F66">
+        <v>525</v>
+      </c>
+      <c r="G66">
+        <v>525</v>
+      </c>
+      <c r="H66">
+        <v>524</v>
+      </c>
+      <c r="I66">
+        <f>AVERAGE(D66:H66)</f>
+        <v>524.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>4071</v>
+      </c>
+      <c r="E67">
+        <v>4116</v>
+      </c>
+      <c r="F67">
+        <v>4149</v>
+      </c>
+      <c r="G67">
+        <v>4134</v>
+      </c>
+      <c r="H67">
+        <v>4119</v>
+      </c>
+      <c r="I67">
+        <f>AVERAGE(D67:H67)</f>
+        <v>4117.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <f>AVERAGE(D68:H68)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="C69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <f>AVERAGE(D69:H69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>2</v>
+      </c>
+      <c r="F72">
+        <v>3</v>
+      </c>
+      <c r="G72">
+        <v>4</v>
+      </c>
+      <c r="H72">
+        <v>5</v>
+      </c>
+      <c r="I72" t="s">
+        <v>4</v>
+      </c>
+      <c r="J72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73">
+        <v>11</v>
+      </c>
+      <c r="B73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>8557</v>
+      </c>
+      <c r="E73">
+        <v>7990</v>
+      </c>
+      <c r="F73">
+        <v>9092</v>
+      </c>
+      <c r="G73">
+        <v>8510</v>
+      </c>
+      <c r="H73">
+        <v>8520</v>
+      </c>
+      <c r="I73">
+        <f>AVERAGE(D73:H73)</f>
+        <v>8533.7999999999993</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="C74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>23207</v>
+      </c>
+      <c r="E74">
+        <v>23138</v>
+      </c>
+      <c r="F74">
+        <v>23229</v>
+      </c>
+      <c r="G74">
+        <v>23289</v>
+      </c>
+      <c r="H74">
+        <v>23727</v>
+      </c>
+      <c r="I74">
+        <f>AVERAGE(D74:H74)</f>
+        <v>23318</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>120</v>
+      </c>
+      <c r="E75">
+        <v>101</v>
+      </c>
+      <c r="F75">
+        <v>120</v>
+      </c>
+      <c r="G75">
+        <v>160</v>
+      </c>
+      <c r="H75">
+        <v>65</v>
+      </c>
+      <c r="I75">
+        <f>AVERAGE(D75:H75)</f>
+        <v>113.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="C76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <v>16</v>
+      </c>
+      <c r="E76">
+        <v>15</v>
+      </c>
+      <c r="F76">
+        <v>16</v>
+      </c>
+      <c r="G76">
+        <v>31</v>
+      </c>
+      <c r="H76">
+        <v>16</v>
+      </c>
+      <c r="I76">
+        <f>AVERAGE(D76:H76)</f>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+      <c r="H79">
+        <v>5</v>
+      </c>
+      <c r="I79" t="s">
+        <v>4</v>
+      </c>
+      <c r="J79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80">
+        <v>12</v>
+      </c>
+      <c r="B80">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>916</v>
+      </c>
+      <c r="E80">
+        <v>944</v>
+      </c>
+      <c r="F80">
+        <v>921</v>
+      </c>
+      <c r="G80">
+        <v>922</v>
+      </c>
+      <c r="H80">
+        <v>916</v>
+      </c>
+      <c r="I80">
+        <f>AVERAGE(D80:H80)</f>
+        <v>923.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="C81" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <v>6206</v>
+      </c>
+      <c r="E81">
+        <v>6364</v>
+      </c>
+      <c r="F81">
+        <v>6255</v>
+      </c>
+      <c r="G81">
+        <v>6903</v>
+      </c>
+      <c r="H81">
+        <v>6224</v>
+      </c>
+      <c r="I81">
+        <f>AVERAGE(D81:H81)</f>
+        <v>6390.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>10</v>
+      </c>
+      <c r="E82">
+        <v>9</v>
+      </c>
+      <c r="F82">
+        <v>8</v>
+      </c>
+      <c r="G82">
+        <v>9</v>
+      </c>
+      <c r="H82">
+        <v>8</v>
+      </c>
+      <c r="I82">
+        <f>AVERAGE(D82:H82)</f>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>16</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>15</v>
+      </c>
+      <c r="G83">
+        <v>16</v>
+      </c>
+      <c r="H83">
+        <v>15</v>
+      </c>
+      <c r="I83">
+        <f>AVERAGE(D83:H83)</f>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86">
+        <v>3</v>
+      </c>
+      <c r="G86">
+        <v>4</v>
+      </c>
+      <c r="H86">
+        <v>5</v>
+      </c>
+      <c r="I86" t="s">
+        <v>4</v>
+      </c>
+      <c r="J86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87">
+        <v>13</v>
+      </c>
+      <c r="B87">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>573</v>
+      </c>
+      <c r="E87">
+        <v>576</v>
+      </c>
+      <c r="F87">
+        <v>571</v>
+      </c>
+      <c r="G87">
+        <v>576</v>
+      </c>
+      <c r="H87">
+        <v>573</v>
+      </c>
+      <c r="I87">
+        <f>AVERAGE(D87:H87)</f>
+        <v>573.79999999999995</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="C88" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>4008</v>
+      </c>
+      <c r="E88">
+        <v>4010</v>
+      </c>
+      <c r="F88">
+        <v>3994</v>
+      </c>
+      <c r="G88">
+        <v>3961</v>
+      </c>
+      <c r="H88">
+        <v>4073</v>
+      </c>
+      <c r="I88">
+        <f>AVERAGE(D88:H88)</f>
+        <v>4009.2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>7</v>
+      </c>
+      <c r="E89">
+        <v>7</v>
+      </c>
+      <c r="F89">
+        <v>6</v>
+      </c>
+      <c r="G89">
+        <v>6</v>
+      </c>
+      <c r="H89">
+        <v>6</v>
+      </c>
+      <c r="I89">
+        <f>AVERAGE(D89:H89)</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="C90" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <v>16</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <f>AVERAGE(D90:H90)</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>4</v>
+      </c>
+      <c r="H93">
+        <v>5</v>
+      </c>
+      <c r="I93" t="s">
+        <v>4</v>
+      </c>
+      <c r="J93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>14</v>
+      </c>
+      <c r="B94">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>482</v>
+      </c>
+      <c r="E94">
+        <v>482</v>
+      </c>
+      <c r="F94">
+        <v>483</v>
+      </c>
+      <c r="G94">
+        <v>482</v>
+      </c>
+      <c r="H94">
+        <v>482</v>
+      </c>
+      <c r="I94">
+        <f>AVERAGE(D94:H94)</f>
+        <v>482.2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>3792</v>
+      </c>
+      <c r="E95">
+        <v>3808</v>
+      </c>
+      <c r="F95">
+        <v>3775</v>
+      </c>
+      <c r="G95">
+        <v>3838</v>
+      </c>
+      <c r="H95">
+        <v>3759</v>
+      </c>
+      <c r="I95">
+        <f>AVERAGE(D95:H95)</f>
+        <v>3794.4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>6</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <v>6</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+      <c r="H96">
+        <v>5</v>
+      </c>
+      <c r="I96">
+        <f>AVERAGE(D96:H96)</f>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="97" spans="3:9">
+      <c r="C97" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>15</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>16</v>
+      </c>
+      <c r="I97">
+        <f>AVERAGE(D97:H97)</f>
         <v>6.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor updates to LBR SQL queries while benchmarking
Testing the timing of the LBR data use case queries.
</commit_message>
<xml_diff>
--- a/usecases/littlebearriver/sqlscripts/QueryBenchmarking.xlsx
+++ b/usecases/littlebearriver/sqlscripts/QueryBenchmarking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23260" yWindow="0" windowWidth="14940" windowHeight="21680" tabRatio="500"/>
+    <workbookView xWindow="-25460" yWindow="0" windowWidth="24060" windowHeight="27520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="8">
   <si>
     <t>Query</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>ODM2 is slower</t>
+  </si>
+  <si>
+    <t>ODM2 is slightly faster</t>
   </si>
 </sst>
 </file>
@@ -490,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="H98" sqref="H98"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -526,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -540,23 +543,23 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>6106</v>
+        <v>1900</v>
       </c>
       <c r="E3">
-        <v>6987</v>
+        <v>1818</v>
       </c>
       <c r="F3">
-        <v>6312</v>
+        <v>1771</v>
       </c>
       <c r="G3">
-        <v>6814</v>
+        <v>2071</v>
       </c>
       <c r="H3">
-        <v>6713</v>
+        <v>1819</v>
       </c>
       <c r="I3">
         <f>AVERAGE(D3:H3)</f>
-        <v>6586.4</v>
+        <v>1875.8</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -564,23 +567,23 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>4227</v>
+        <v>4289</v>
       </c>
       <c r="E4">
-        <v>4242</v>
+        <v>4243</v>
       </c>
       <c r="F4">
-        <v>4476</v>
+        <v>4167</v>
       </c>
       <c r="G4">
-        <v>4197</v>
+        <v>4244</v>
       </c>
       <c r="H4">
-        <v>4103</v>
+        <v>4260</v>
       </c>
       <c r="I4">
         <f>AVERAGE(D4:H4)</f>
-        <v>4249</v>
+        <v>4240.6000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -591,23 +594,23 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>5557</v>
+        <v>1721</v>
       </c>
       <c r="E5">
-        <v>4891</v>
+        <v>1853</v>
       </c>
       <c r="F5">
-        <v>4461</v>
+        <v>1763</v>
       </c>
       <c r="G5">
-        <v>5668</v>
+        <v>1874</v>
       </c>
       <c r="H5">
-        <v>5357</v>
+        <v>1640</v>
       </c>
       <c r="I5">
         <f>AVERAGE(D5:H5)</f>
-        <v>5186.8</v>
+        <v>1770.2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -615,23 +618,23 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>3401</v>
+        <v>4102</v>
       </c>
       <c r="E6">
-        <v>3667</v>
+        <v>4199</v>
       </c>
       <c r="F6">
-        <v>3713</v>
+        <v>4273</v>
       </c>
       <c r="G6">
-        <v>3710</v>
+        <v>4119</v>
       </c>
       <c r="H6">
-        <v>3574</v>
+        <v>4352</v>
       </c>
       <c r="I6">
         <f>AVERAGE(D6:H6)</f>
-        <v>3613</v>
+        <v>4209</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -660,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -674,23 +677,23 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>682</v>
+        <v>491</v>
       </c>
       <c r="E10">
-        <v>646</v>
+        <v>491</v>
       </c>
       <c r="F10">
-        <v>819</v>
+        <v>490</v>
       </c>
       <c r="G10">
-        <v>733</v>
+        <v>491</v>
       </c>
       <c r="H10">
-        <v>855</v>
+        <v>490</v>
       </c>
       <c r="I10">
         <f>AVERAGE(D10:H10)</f>
-        <v>747</v>
+        <v>490.6</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -698,23 +701,23 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>3617</v>
+        <v>3884</v>
       </c>
       <c r="E11">
-        <v>3993</v>
+        <v>3961</v>
       </c>
       <c r="F11">
-        <v>3870</v>
+        <v>3869</v>
       </c>
       <c r="G11">
-        <v>3778</v>
+        <v>3902</v>
       </c>
       <c r="H11">
-        <v>4024</v>
+        <v>3882</v>
       </c>
       <c r="I11">
         <f>AVERAGE(D11:H11)</f>
-        <v>3856.4</v>
+        <v>3899.6</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -725,23 +728,23 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>967</v>
+        <v>493</v>
       </c>
       <c r="E12">
-        <v>932</v>
+        <v>459</v>
       </c>
       <c r="F12">
-        <v>961</v>
+        <v>457</v>
       </c>
       <c r="G12">
-        <v>1076</v>
+        <v>457</v>
       </c>
       <c r="H12">
-        <v>1431</v>
+        <v>457</v>
       </c>
       <c r="I12">
         <f>AVERAGE(D12:H12)</f>
-        <v>1073.4000000000001</v>
+        <v>464.6</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -749,23 +752,23 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>3353</v>
+        <v>3605</v>
       </c>
       <c r="E13">
-        <v>2931</v>
+        <v>3632</v>
       </c>
       <c r="F13">
-        <v>3090</v>
+        <v>3619</v>
       </c>
       <c r="G13">
-        <v>2949</v>
+        <v>3621</v>
       </c>
       <c r="H13">
-        <v>2838</v>
+        <v>3633</v>
       </c>
       <c r="I13">
         <f>AVERAGE(D13:H13)</f>
-        <v>3032.2</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -808,23 +811,23 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="E17">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="F17">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="G17">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="H17">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="I17">
         <f>AVERAGE(D17:H17)</f>
-        <v>477.2</v>
+        <v>488.6</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -832,23 +835,23 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>3776</v>
+        <v>3868</v>
       </c>
       <c r="E18">
-        <v>3775</v>
+        <v>3870</v>
       </c>
       <c r="F18">
-        <v>3792</v>
+        <v>3883</v>
       </c>
       <c r="G18">
-        <v>3744</v>
+        <v>3869</v>
       </c>
       <c r="H18">
-        <v>3744</v>
+        <v>3852</v>
       </c>
       <c r="I18">
         <f>AVERAGE(D18:H18)</f>
-        <v>3766.2</v>
+        <v>3868.4</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -859,23 +862,23 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="G19">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="H19">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="I19">
         <f>AVERAGE(D19:H19)</f>
-        <v>5.4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -883,23 +886,23 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F20">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="I20">
         <f>AVERAGE(D20:H20)</f>
-        <v>3</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -993,23 +996,23 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I26">
         <f>AVERAGE(D26:H26)</f>
-        <v>9.4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1017,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>15</v>
@@ -1033,7 +1036,7 @@
       </c>
       <c r="I27">
         <f>AVERAGE(D27:H27)</f>
-        <v>6.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1127,23 +1130,23 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F33">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G33">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H33">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I33">
         <f>AVERAGE(D33:H33)</f>
-        <v>9.8000000000000007</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1154,20 +1157,20 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G34">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <f>AVERAGE(D34:H34)</f>
-        <v>9.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1261,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -1277,7 +1280,7 @@
       </c>
       <c r="I40">
         <f>AVERAGE(D40:H40)</f>
-        <v>4.2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1291,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1301,7 +1304,7 @@
       </c>
       <c r="I41">
         <f>AVERAGE(D41:H41)</f>
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1395,7 +1398,7 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E47">
         <v>13</v>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="I47">
         <f>AVERAGE(D47:H47)</f>
-        <v>13.8</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1419,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="D48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -1435,7 +1438,7 @@
       </c>
       <c r="I48">
         <f>AVERAGE(D48:H48)</f>
-        <v>15.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -1464,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="J51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -1478,23 +1481,23 @@
         <v>2</v>
       </c>
       <c r="D52">
-        <v>89765</v>
+        <v>519</v>
       </c>
       <c r="E52">
-        <v>89800</v>
+        <v>518</v>
       </c>
       <c r="F52">
-        <v>89710</v>
+        <v>519</v>
       </c>
       <c r="G52">
-        <v>282219</v>
+        <v>520</v>
       </c>
       <c r="H52">
-        <v>278291</v>
+        <v>519</v>
       </c>
       <c r="I52">
         <f>AVERAGE(D52:H52)</f>
-        <v>165957</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -1502,23 +1505,23 @@
         <v>3</v>
       </c>
       <c r="D53">
-        <v>89763</v>
+        <v>4087</v>
       </c>
       <c r="E53">
-        <v>89779</v>
+        <v>4118</v>
       </c>
       <c r="F53">
-        <v>89653</v>
+        <v>4118</v>
       </c>
       <c r="G53">
-        <v>143302</v>
+        <v>4119</v>
       </c>
       <c r="H53">
-        <v>142866</v>
+        <v>4119</v>
       </c>
       <c r="I53">
         <f>AVERAGE(D53:H53)</f>
-        <v>111072.6</v>
+        <v>4112.2</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -1529,23 +1532,23 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <v>234</v>
+        <v>1583</v>
       </c>
       <c r="E54">
-        <v>231</v>
+        <v>1584</v>
       </c>
       <c r="F54">
-        <v>227</v>
+        <v>1585</v>
       </c>
       <c r="G54">
-        <v>214</v>
+        <v>1583</v>
       </c>
       <c r="H54">
-        <v>214</v>
+        <v>1584</v>
       </c>
       <c r="I54">
         <f>AVERAGE(D54:H54)</f>
-        <v>224</v>
+        <v>1583.8</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -1553,23 +1556,23 @@
         <v>3</v>
       </c>
       <c r="D55">
-        <v>187</v>
+        <v>1576</v>
       </c>
       <c r="E55">
-        <v>124</v>
+        <v>1575</v>
       </c>
       <c r="F55">
-        <v>125</v>
+        <v>1576</v>
       </c>
       <c r="G55">
-        <v>156</v>
+        <v>1591</v>
       </c>
       <c r="H55">
-        <v>78</v>
+        <v>1576</v>
       </c>
       <c r="I55">
         <f>AVERAGE(D55:H55)</f>
-        <v>134</v>
+        <v>1578.8</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -1663,23 +1666,23 @@
         <v>2</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="E61">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="F61">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="G61">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="H61">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="I61">
         <f>AVERAGE(D61:H61)</f>
-        <v>3.2</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -1687,23 +1690,23 @@
         <v>3</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="G62">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="I62">
         <f>AVERAGE(D62:H62)</f>
-        <v>3.2</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -1746,23 +1749,23 @@
         <v>2</v>
       </c>
       <c r="D66">
-        <v>524</v>
+        <v>504</v>
       </c>
       <c r="E66">
-        <v>525</v>
+        <v>503</v>
       </c>
       <c r="F66">
-        <v>525</v>
+        <v>506</v>
       </c>
       <c r="G66">
-        <v>525</v>
+        <v>506</v>
       </c>
       <c r="H66">
-        <v>524</v>
+        <v>505</v>
       </c>
       <c r="I66">
         <f>AVERAGE(D66:H66)</f>
-        <v>524.6</v>
+        <v>504.8</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -1770,23 +1773,23 @@
         <v>3</v>
       </c>
       <c r="D67">
-        <v>4071</v>
+        <v>4009</v>
       </c>
       <c r="E67">
-        <v>4116</v>
+        <v>3977</v>
       </c>
       <c r="F67">
-        <v>4149</v>
+        <v>4025</v>
       </c>
       <c r="G67">
-        <v>4134</v>
+        <v>3978</v>
       </c>
       <c r="H67">
-        <v>4119</v>
+        <v>3979</v>
       </c>
       <c r="I67">
         <f>AVERAGE(D67:H67)</f>
-        <v>4117.8</v>
+        <v>3993.6</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -1797,23 +1800,23 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I68">
         <f>AVERAGE(D68:H68)</f>
-        <v>0.4</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -1824,20 +1827,20 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
         <f>AVERAGE(D69:H69)</f>
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -1880,23 +1883,23 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>8557</v>
+        <v>3819</v>
       </c>
       <c r="E73">
-        <v>7990</v>
+        <v>3772</v>
       </c>
       <c r="F73">
-        <v>9092</v>
+        <v>3569</v>
       </c>
       <c r="G73">
-        <v>8510</v>
+        <v>3593</v>
       </c>
       <c r="H73">
-        <v>8520</v>
+        <v>3760</v>
       </c>
       <c r="I73">
         <f>AVERAGE(D73:H73)</f>
-        <v>8533.7999999999993</v>
+        <v>3702.6</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -1904,23 +1907,23 @@
         <v>3</v>
       </c>
       <c r="D74">
-        <v>23207</v>
+        <v>24550</v>
       </c>
       <c r="E74">
-        <v>23138</v>
+        <v>24398</v>
       </c>
       <c r="F74">
-        <v>23229</v>
+        <v>24370</v>
       </c>
       <c r="G74">
-        <v>23289</v>
+        <v>24272</v>
       </c>
       <c r="H74">
-        <v>23727</v>
+        <v>24402</v>
       </c>
       <c r="I74">
         <f>AVERAGE(D74:H74)</f>
-        <v>23318</v>
+        <v>24398.400000000001</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -1931,23 +1934,23 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>120</v>
+        <v>38</v>
       </c>
       <c r="E75">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="F75">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="G75">
-        <v>160</v>
+        <v>28</v>
       </c>
       <c r="H75">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="I75">
         <f>AVERAGE(D75:H75)</f>
-        <v>113.2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -1955,23 +1958,23 @@
         <v>3</v>
       </c>
       <c r="D76">
+        <v>15</v>
+      </c>
+      <c r="E76">
         <v>16</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>15</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>16</v>
       </c>
-      <c r="G76">
-        <v>31</v>
-      </c>
       <c r="H76">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I76">
         <f>AVERAGE(D76:H76)</f>
-        <v>18.8</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2065,23 +2068,23 @@
         <v>2</v>
       </c>
       <c r="D82">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E82">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F82">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G82">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H82">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I82">
         <f>AVERAGE(D82:H82)</f>
-        <v>8.8000000000000007</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -2092,7 +2095,7 @@
         <v>16</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F83">
         <v>15</v>
@@ -2105,7 +2108,7 @@
       </c>
       <c r="I83">
         <f>AVERAGE(D83:H83)</f>
-        <v>12.4</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -2199,23 +2202,23 @@
         <v>2</v>
       </c>
       <c r="D89">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E89">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="F89">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="G89">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="H89">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="I89">
         <f>AVERAGE(D89:H89)</f>
-        <v>6.4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -2223,23 +2226,23 @@
         <v>3</v>
       </c>
       <c r="D90">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E90">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="I90">
         <f>AVERAGE(D90:H90)</f>
-        <v>6.4</v>
+        <v>62.6</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -2333,23 +2336,23 @@
         <v>2</v>
       </c>
       <c r="D96">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E96">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F96">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G96">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H96">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="I96">
         <f>AVERAGE(D96:H96)</f>
-        <v>5.4</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="97" spans="3:9">
@@ -2357,23 +2360,23 @@
         <v>3</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F97">
+        <v>16</v>
+      </c>
+      <c r="G97">
         <v>15</v>
-      </c>
-      <c r="G97">
-        <v>0</v>
       </c>
       <c r="H97">
         <v>16</v>
       </c>
       <c r="I97">
         <f>AVERAGE(D97:H97)</f>
-        <v>6.2</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rolling back the stuff I did tonight
DBWrench XML sucks.  I have spent hours trying to resolve the
differences between the XML files and have been unsuccessful.  I will
be better off just redoing the provenance features in a new feature
branch based on the master and then merging it back in.
</commit_message>
<xml_diff>
--- a/usecases/littlebearriver/sqlscripts/QueryBenchmarking.xlsx
+++ b/usecases/littlebearriver/sqlscripts/QueryBenchmarking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25460" yWindow="0" windowWidth="24060" windowHeight="27520" tabRatio="500"/>
+    <workbookView xWindow="23260" yWindow="0" windowWidth="14940" windowHeight="21680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="7">
   <si>
     <t>Query</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>ODM2 is slower</t>
-  </si>
-  <si>
-    <t>ODM2 is slightly faster</t>
   </si>
 </sst>
 </file>
@@ -493,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -529,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -543,23 +540,23 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1900</v>
+        <v>6106</v>
       </c>
       <c r="E3">
-        <v>1818</v>
+        <v>6987</v>
       </c>
       <c r="F3">
-        <v>1771</v>
+        <v>6312</v>
       </c>
       <c r="G3">
-        <v>2071</v>
+        <v>6814</v>
       </c>
       <c r="H3">
-        <v>1819</v>
+        <v>6713</v>
       </c>
       <c r="I3">
         <f>AVERAGE(D3:H3)</f>
-        <v>1875.8</v>
+        <v>6586.4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -567,23 +564,23 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>4289</v>
+        <v>4227</v>
       </c>
       <c r="E4">
-        <v>4243</v>
+        <v>4242</v>
       </c>
       <c r="F4">
-        <v>4167</v>
+        <v>4476</v>
       </c>
       <c r="G4">
-        <v>4244</v>
+        <v>4197</v>
       </c>
       <c r="H4">
-        <v>4260</v>
+        <v>4103</v>
       </c>
       <c r="I4">
         <f>AVERAGE(D4:H4)</f>
-        <v>4240.6000000000004</v>
+        <v>4249</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -594,23 +591,23 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>1721</v>
+        <v>5557</v>
       </c>
       <c r="E5">
-        <v>1853</v>
+        <v>4891</v>
       </c>
       <c r="F5">
-        <v>1763</v>
+        <v>4461</v>
       </c>
       <c r="G5">
-        <v>1874</v>
+        <v>5668</v>
       </c>
       <c r="H5">
-        <v>1640</v>
+        <v>5357</v>
       </c>
       <c r="I5">
         <f>AVERAGE(D5:H5)</f>
-        <v>1770.2</v>
+        <v>5186.8</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -618,23 +615,23 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>4102</v>
+        <v>3401</v>
       </c>
       <c r="E6">
-        <v>4199</v>
+        <v>3667</v>
       </c>
       <c r="F6">
-        <v>4273</v>
+        <v>3713</v>
       </c>
       <c r="G6">
-        <v>4119</v>
+        <v>3710</v>
       </c>
       <c r="H6">
-        <v>4352</v>
+        <v>3574</v>
       </c>
       <c r="I6">
         <f>AVERAGE(D6:H6)</f>
-        <v>4209</v>
+        <v>3613</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -663,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -677,23 +674,23 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>491</v>
+        <v>682</v>
       </c>
       <c r="E10">
-        <v>491</v>
+        <v>646</v>
       </c>
       <c r="F10">
-        <v>490</v>
+        <v>819</v>
       </c>
       <c r="G10">
-        <v>491</v>
+        <v>733</v>
       </c>
       <c r="H10">
-        <v>490</v>
+        <v>855</v>
       </c>
       <c r="I10">
         <f>AVERAGE(D10:H10)</f>
-        <v>490.6</v>
+        <v>747</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -701,23 +698,23 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>3884</v>
+        <v>3617</v>
       </c>
       <c r="E11">
-        <v>3961</v>
+        <v>3993</v>
       </c>
       <c r="F11">
-        <v>3869</v>
+        <v>3870</v>
       </c>
       <c r="G11">
-        <v>3902</v>
+        <v>3778</v>
       </c>
       <c r="H11">
-        <v>3882</v>
+        <v>4024</v>
       </c>
       <c r="I11">
         <f>AVERAGE(D11:H11)</f>
-        <v>3899.6</v>
+        <v>3856.4</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -728,23 +725,23 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>493</v>
+        <v>967</v>
       </c>
       <c r="E12">
-        <v>459</v>
+        <v>932</v>
       </c>
       <c r="F12">
-        <v>457</v>
+        <v>961</v>
       </c>
       <c r="G12">
-        <v>457</v>
+        <v>1076</v>
       </c>
       <c r="H12">
-        <v>457</v>
+        <v>1431</v>
       </c>
       <c r="I12">
         <f>AVERAGE(D12:H12)</f>
-        <v>464.6</v>
+        <v>1073.4000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -752,23 +749,23 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>3605</v>
+        <v>3353</v>
       </c>
       <c r="E13">
-        <v>3632</v>
+        <v>2931</v>
       </c>
       <c r="F13">
-        <v>3619</v>
+        <v>3090</v>
       </c>
       <c r="G13">
-        <v>3621</v>
+        <v>2949</v>
       </c>
       <c r="H13">
-        <v>3633</v>
+        <v>2838</v>
       </c>
       <c r="I13">
         <f>AVERAGE(D13:H13)</f>
-        <v>3622</v>
+        <v>3032.2</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -811,23 +808,23 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="E17">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="F17">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="G17">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="H17">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="I17">
         <f>AVERAGE(D17:H17)</f>
-        <v>488.6</v>
+        <v>477.2</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -835,23 +832,23 @@
         <v>3</v>
       </c>
       <c r="D18">
-        <v>3868</v>
+        <v>3776</v>
       </c>
       <c r="E18">
-        <v>3870</v>
+        <v>3775</v>
       </c>
       <c r="F18">
-        <v>3883</v>
+        <v>3792</v>
       </c>
       <c r="G18">
-        <v>3869</v>
+        <v>3744</v>
       </c>
       <c r="H18">
-        <v>3852</v>
+        <v>3744</v>
       </c>
       <c r="I18">
         <f>AVERAGE(D18:H18)</f>
-        <v>3868.4</v>
+        <v>3766.2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -862,23 +859,23 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="F19">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="G19">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="I19">
         <f>AVERAGE(D19:H19)</f>
-        <v>41</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -886,23 +883,23 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <f>AVERAGE(D20:H20)</f>
-        <v>43.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -996,23 +993,23 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H26">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I26">
         <f>AVERAGE(D26:H26)</f>
-        <v>12</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1020,7 +1017,7 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E27">
         <v>15</v>
@@ -1036,7 +1033,7 @@
       </c>
       <c r="I27">
         <f>AVERAGE(D27:H27)</f>
-        <v>3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1130,23 +1127,23 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E33">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F33">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G33">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H33">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I33">
         <f>AVERAGE(D33:H33)</f>
-        <v>6.8</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1157,20 +1154,20 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>16</v>
+      </c>
+      <c r="H34">
         <v>15</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
       </c>
       <c r="I34">
         <f>AVERAGE(D34:H34)</f>
-        <v>3</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1264,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -1280,7 +1277,7 @@
       </c>
       <c r="I40">
         <f>AVERAGE(D40:H40)</f>
-        <v>1.8</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1294,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1304,7 +1301,7 @@
       </c>
       <c r="I41">
         <f>AVERAGE(D41:H41)</f>
-        <v>3.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1398,7 +1395,7 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E47">
         <v>13</v>
@@ -1414,7 +1411,7 @@
       </c>
       <c r="I47">
         <f>AVERAGE(D47:H47)</f>
-        <v>18.8</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1422,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E48">
         <v>15</v>
@@ -1438,7 +1435,7 @@
       </c>
       <c r="I48">
         <f>AVERAGE(D48:H48)</f>
-        <v>12.4</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -1467,7 +1464,7 @@
         <v>4</v>
       </c>
       <c r="J51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -1481,23 +1478,23 @@
         <v>2</v>
       </c>
       <c r="D52">
-        <v>519</v>
+        <v>89765</v>
       </c>
       <c r="E52">
-        <v>518</v>
+        <v>89800</v>
       </c>
       <c r="F52">
-        <v>519</v>
+        <v>89710</v>
       </c>
       <c r="G52">
-        <v>520</v>
+        <v>282219</v>
       </c>
       <c r="H52">
-        <v>519</v>
+        <v>278291</v>
       </c>
       <c r="I52">
         <f>AVERAGE(D52:H52)</f>
-        <v>519</v>
+        <v>165957</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -1505,23 +1502,23 @@
         <v>3</v>
       </c>
       <c r="D53">
-        <v>4087</v>
+        <v>89763</v>
       </c>
       <c r="E53">
-        <v>4118</v>
+        <v>89779</v>
       </c>
       <c r="F53">
-        <v>4118</v>
+        <v>89653</v>
       </c>
       <c r="G53">
-        <v>4119</v>
+        <v>143302</v>
       </c>
       <c r="H53">
-        <v>4119</v>
+        <v>142866</v>
       </c>
       <c r="I53">
         <f>AVERAGE(D53:H53)</f>
-        <v>4112.2</v>
+        <v>111072.6</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -1532,23 +1529,23 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <v>1583</v>
+        <v>234</v>
       </c>
       <c r="E54">
-        <v>1584</v>
+        <v>231</v>
       </c>
       <c r="F54">
-        <v>1585</v>
+        <v>227</v>
       </c>
       <c r="G54">
-        <v>1583</v>
+        <v>214</v>
       </c>
       <c r="H54">
-        <v>1584</v>
+        <v>214</v>
       </c>
       <c r="I54">
         <f>AVERAGE(D54:H54)</f>
-        <v>1583.8</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -1556,23 +1553,23 @@
         <v>3</v>
       </c>
       <c r="D55">
-        <v>1576</v>
+        <v>187</v>
       </c>
       <c r="E55">
-        <v>1575</v>
+        <v>124</v>
       </c>
       <c r="F55">
-        <v>1576</v>
+        <v>125</v>
       </c>
       <c r="G55">
-        <v>1591</v>
+        <v>156</v>
       </c>
       <c r="H55">
-        <v>1576</v>
+        <v>78</v>
       </c>
       <c r="I55">
         <f>AVERAGE(D55:H55)</f>
-        <v>1578.8</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -1666,23 +1663,23 @@
         <v>2</v>
       </c>
       <c r="D61">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E61">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="G61">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="H61">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="I61">
         <f>AVERAGE(D61:H61)</f>
-        <v>57.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -1690,23 +1687,23 @@
         <v>3</v>
       </c>
       <c r="D62">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="H62">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="I62">
         <f>AVERAGE(D62:H62)</f>
-        <v>56.2</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -1749,23 +1746,23 @@
         <v>2</v>
       </c>
       <c r="D66">
-        <v>504</v>
+        <v>524</v>
       </c>
       <c r="E66">
-        <v>503</v>
+        <v>525</v>
       </c>
       <c r="F66">
-        <v>506</v>
+        <v>525</v>
       </c>
       <c r="G66">
-        <v>506</v>
+        <v>525</v>
       </c>
       <c r="H66">
-        <v>505</v>
+        <v>524</v>
       </c>
       <c r="I66">
         <f>AVERAGE(D66:H66)</f>
-        <v>504.8</v>
+        <v>524.6</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -1773,23 +1770,23 @@
         <v>3</v>
       </c>
       <c r="D67">
-        <v>4009</v>
+        <v>4071</v>
       </c>
       <c r="E67">
-        <v>3977</v>
+        <v>4116</v>
       </c>
       <c r="F67">
-        <v>4025</v>
+        <v>4149</v>
       </c>
       <c r="G67">
-        <v>3978</v>
+        <v>4134</v>
       </c>
       <c r="H67">
-        <v>3979</v>
+        <v>4119</v>
       </c>
       <c r="I67">
         <f>AVERAGE(D67:H67)</f>
-        <v>3993.6</v>
+        <v>4117.8</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -1800,23 +1797,23 @@
         <v>2</v>
       </c>
       <c r="D68">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H68">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I68">
         <f>AVERAGE(D68:H68)</f>
-        <v>6.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -1827,20 +1824,20 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
         <f>AVERAGE(D69:H69)</f>
-        <v>6.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -1883,23 +1880,23 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>3819</v>
+        <v>8557</v>
       </c>
       <c r="E73">
-        <v>3772</v>
+        <v>7990</v>
       </c>
       <c r="F73">
-        <v>3569</v>
+        <v>9092</v>
       </c>
       <c r="G73">
-        <v>3593</v>
+        <v>8510</v>
       </c>
       <c r="H73">
-        <v>3760</v>
+        <v>8520</v>
       </c>
       <c r="I73">
         <f>AVERAGE(D73:H73)</f>
-        <v>3702.6</v>
+        <v>8533.7999999999993</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -1907,23 +1904,23 @@
         <v>3</v>
       </c>
       <c r="D74">
-        <v>24550</v>
+        <v>23207</v>
       </c>
       <c r="E74">
-        <v>24398</v>
+        <v>23138</v>
       </c>
       <c r="F74">
-        <v>24370</v>
+        <v>23229</v>
       </c>
       <c r="G74">
-        <v>24272</v>
+        <v>23289</v>
       </c>
       <c r="H74">
-        <v>24402</v>
+        <v>23727</v>
       </c>
       <c r="I74">
         <f>AVERAGE(D74:H74)</f>
-        <v>24398.400000000001</v>
+        <v>23318</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -1934,23 +1931,23 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="E75">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="F75">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="G75">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="H75">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="I75">
         <f>AVERAGE(D75:H75)</f>
-        <v>30</v>
+        <v>113.2</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -1958,23 +1955,23 @@
         <v>3</v>
       </c>
       <c r="D76">
+        <v>16</v>
+      </c>
+      <c r="E76">
         <v>15</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>16</v>
       </c>
-      <c r="F76">
-        <v>15</v>
-      </c>
       <c r="G76">
+        <v>31</v>
+      </c>
+      <c r="H76">
         <v>16</v>
-      </c>
-      <c r="H76">
-        <v>15</v>
       </c>
       <c r="I76">
         <f>AVERAGE(D76:H76)</f>
-        <v>15.4</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2068,23 +2065,23 @@
         <v>2</v>
       </c>
       <c r="D82">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E82">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F82">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G82">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H82">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I82">
         <f>AVERAGE(D82:H82)</f>
-        <v>14.2</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -2095,7 +2092,7 @@
         <v>16</v>
       </c>
       <c r="E83">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F83">
         <v>15</v>
@@ -2108,7 +2105,7 @@
       </c>
       <c r="I83">
         <f>AVERAGE(D83:H83)</f>
-        <v>15.6</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -2202,23 +2199,23 @@
         <v>2</v>
       </c>
       <c r="D89">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E89">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="F89">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="G89">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="H89">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="I89">
         <f>AVERAGE(D89:H89)</f>
-        <v>62</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -2226,23 +2223,23 @@
         <v>3</v>
       </c>
       <c r="D90">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="E90">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="F90">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="I90">
         <f>AVERAGE(D90:H90)</f>
-        <v>62.6</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -2336,23 +2333,23 @@
         <v>2</v>
       </c>
       <c r="D96">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E96">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F96">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G96">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="H96">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I96">
         <f>AVERAGE(D96:H96)</f>
-        <v>17.2</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="97" spans="3:9">
@@ -2360,23 +2357,23 @@
         <v>3</v>
       </c>
       <c r="D97">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
         <v>15</v>
       </c>
-      <c r="F97">
-        <v>16</v>
-      </c>
       <c r="G97">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H97">
         <v>16</v>
       </c>
       <c r="I97">
         <f>AVERAGE(D97:H97)</f>
-        <v>18.600000000000001</v>
+        <v>6.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>